<commit_message>
right graph for resnet 101 10gbps, in rack, even, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_even_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/10gbps_inrack_even_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -264,16 +261,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2617</c:v>
+                    <c:v>0.2552</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.6523</c:v>
+                    <c:v>3.508</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.9735</c:v>
+                    <c:v>1.7932</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.8986</c:v>
+                    <c:v>1.2095</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0103</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8581</c:v>
+                    <c:v>0.8217</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>5.5888</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9171</c:v>
+                    <c:v>2.4743</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1651</c:v>
+                    <c:v>0.4476</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.2381</c:v>
+                  <c:v>16.8057</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>39.0169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.7652</c:v>
+                  <c:v>39.7396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.6539</c:v>
+                  <c:v>43.6874</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1921</c:v>
+                    <c:v>0.235</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1355</c:v>
+                    <c:v>0.0393</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1415</c:v>
+                    <c:v>7.1593</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.6681</c:v>
+                    <c:v>5.4944</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.649</c:v>
+                    <c:v>1.7789</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.263</c:v>
+                    <c:v>0.0589</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.013</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.9111</c:v>
+                    <c:v>11.4278</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.628</c:v>
+                    <c:v>4.5725</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7959</c:v>
+                    <c:v>2.6209</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -500,13 +497,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.8875</c:v>
+                  <c:v>28.0718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.7256</c:v>
+                  <c:v>27.957</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.3672</c:v>
+                  <c:v>36.6909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1724</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2678</c:v>
+                    <c:v>0.5735</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>14.3773</c:v>
+                    <c:v>12.0045</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.9256</c:v>
+                    <c:v>17.5504</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1141</c:v>
+                    <c:v>1.394</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -582,16 +579,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2434</c:v>
+                    <c:v>0.2871</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.0201</c:v>
+                    <c:v>6.9204</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3723</c:v>
+                    <c:v>3.3494</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.7352</c:v>
+                    <c:v>6.0859</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -647,13 +644,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0201</c:v>
+                  <c:v>6.9204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.482</c:v>
+                  <c:v>0.6707</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.3588</c:v>
+                  <c:v>24.1439</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -708,13 +705,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2197</c:v>
+                    <c:v>0.1325</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>46.4124</c:v>
+                    <c:v>23.681</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>10.6103</c:v>
+                    <c:v>7.43</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -729,16 +726,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1153</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2611</c:v>
+                    <c:v>0.3061</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.0138</c:v>
+                    <c:v>13.604</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.6492</c:v>
+                    <c:v>3.9686</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -794,13 +791,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0286</c:v>
+                  <c:v>0.0372</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-22.6302</c:v>
+                  <c:v>-12.3267</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1264</c:v>
+                  <c:v>0.9135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079145712"/>
-        <c:axId val="-2080476800"/>
+        <c:axId val="-2077313248"/>
+        <c:axId val="-2077306992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079145712"/>
+        <c:axId val="-2077313248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080476800"/>
+        <c:crossAx val="-2077306992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080476800"/>
+        <c:axId val="-2077306992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079145712"/>
+        <c:crossAx val="-2077313248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1073</c:v>
+                    <c:v>1.3318</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0104</c:v>
+                    <c:v>0.0292</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.453</c:v>
+                    <c:v>0.996</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5098</c:v>
+                    <c:v>0.6531</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5275</c:v>
+                    <c:v>0.2646</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0141</c:v>
+                    <c:v>0.0104</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0897</c:v>
+                    <c:v>0.3433</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6045</c:v>
+                    <c:v>0.4973</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.8346</c:v>
+                  <c:v>10.8982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.9838</c:v>
+                  <c:v>27.0252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.9732</c:v>
+                  <c:v>37.5782</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.0756</c:v>
+                  <c:v>44.1259</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.8169</c:v>
+                  <c:v>47.2642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0773</c:v>
+                    <c:v>0.0705</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1272</c:v>
+                    <c:v>0.0882</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1087</c:v>
+                    <c:v>0.0085</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6431</c:v>
+                    <c:v>0.7913</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3704</c:v>
+                    <c:v>0.3835</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1959</c:v>
+                    <c:v>0.0367</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0379</c:v>
+                    <c:v>0.1606</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1396</c:v>
+                    <c:v>0.2354</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1557</c:v>
+                    <c:v>0.2508</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1374</c:v>
+                    <c:v>0.3159</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3841</c:v>
+                  <c:v>0.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0045</c:v>
+                  <c:v>13.8269</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.9838</c:v>
+                  <c:v>27.1244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.9339</c:v>
+                  <c:v>37.565</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.1629</c:v>
+                  <c:v>43.8327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1724</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2636</c:v>
+                    <c:v>0.5732</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7445</c:v>
+                    <c:v>0.0992</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.7588</c:v>
+                    <c:v>1.1251</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2809</c:v>
+                    <c:v>0.1123</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1614,16 +1611,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0286</c:v>
+                    <c:v>0.0037</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1909</c:v>
+                    <c:v>1.8052</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>12.7317</c:v>
+                    <c:v>1.1657</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4184</c:v>
+                    <c:v>0.5371</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1679,13 +1676,13 @@
                   <c:v>0.272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.7415</c:v>
+                  <c:v>15.5781</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.6325</c:v>
+                  <c:v>27.2564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0954</c:v>
+                  <c:v>37.8599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1740,13 +1737,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4064</c:v>
+                    <c:v>0.1693</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.8691</c:v>
+                    <c:v>6.5406</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1304</c:v>
+                    <c:v>7.7695</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1764,13 +1761,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0929</c:v>
+                    <c:v>0.1028</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>42.8665</c:v>
+                    <c:v>22.5865</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.0969</c:v>
+                    <c:v>1.1905</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1826,13 +1823,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3356</c:v>
+                  <c:v>0.3586</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.2014</c:v>
+                  <c:v>8.2473</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.2599</c:v>
+                  <c:v>26.9671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094744352"/>
-        <c:axId val="-2080336400"/>
+        <c:axId val="-2078061712"/>
+        <c:axId val="-2078067968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094744352"/>
+        <c:axId val="-2078061712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080336400"/>
+        <c:crossAx val="-2078067968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080336400"/>
+        <c:axId val="-2078067968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094744352"/>
+        <c:crossAx val="-2078061712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1073</c:v>
+                    <c:v>1.3318</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2618</c:v>
+                    <c:v>0.2553</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.3758</c:v>
+                    <c:v>3.6374</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.26</c:v>
+                    <c:v>4.4547</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8908</c:v>
+                    <c:v>0.7824</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5275</c:v>
+                    <c:v>0.2646</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8388</c:v>
+                    <c:v>0.8094</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.5889</c:v>
+                    <c:v>5.5932</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.9379</c:v>
+                    <c:v>3.3204</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.6204</c:v>
+                    <c:v>0.2583</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-3.8346</c:v>
+                  <c:v>10.8982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.2218</c:v>
+                  <c:v>43.8393</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.9902</c:v>
+                  <c:v>76.5995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.341</c:v>
+                  <c:v>81.0579</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.1139</c:v>
+                  <c:v>90.5021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0773</c:v>
+                    <c:v>0.0705</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1272</c:v>
+                    <c:v>0.0882</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.172</c:v>
+                    <c:v>7.1141</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.6044</c:v>
+                    <c:v>8.3497</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.026</c:v>
+                    <c:v>1.1585</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1959</c:v>
+                    <c:v>0.0367</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0379</c:v>
+                    <c:v>0.1606</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>11.8719</c:v>
+                    <c:v>11.4447</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.6685</c:v>
+                    <c:v>1.1454</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.2532</c:v>
+                    <c:v>0.6332</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3841</c:v>
+                  <c:v>0.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0045</c:v>
+                  <c:v>13.8269</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.832</c:v>
+                  <c:v>55.1055</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.2518</c:v>
+                  <c:v>62.1858</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.2187</c:v>
+                  <c:v>81.07089999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1724</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2636</c:v>
+                    <c:v>0.5732</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>14.3772</c:v>
+                    <c:v>12.0412</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>14.5567</c:v>
+                    <c:v>16.7393</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.7352</c:v>
+                    <c:v>7.6781</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2646,16 +2643,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0286</c:v>
+                    <c:v>0.0037</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.2564</c:v>
+                    <c:v>8.7073</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.8856</c:v>
+                    <c:v>13.6262</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.1136</c:v>
+                    <c:v>1.6013</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2711,13 +2708,13 @@
                   <c:v>0.272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2519</c:v>
+                  <c:v>22.4802</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.0737</c:v>
+                  <c:v>28.4252</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61.6425</c:v>
+                  <c:v>63.0068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2772,13 +2769,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4064</c:v>
+                    <c:v>0.1693</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>45.946</c:v>
+                    <c:v>20.1703</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.4873</c:v>
+                    <c:v>10.4669</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2796,13 +2793,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0929</c:v>
+                    <c:v>0.1028</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>21.0212</c:v>
+                    <c:v>8.7212</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>11.7506</c:v>
+                    <c:v>5.2018</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2858,13 +2855,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3356</c:v>
+                  <c:v>0.3586</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-15.5347</c:v>
+                  <c:v>-5.5627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.5191</c:v>
+                  <c:v>32.331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2078906496"/>
-        <c:axId val="-2078953424"/>
+        <c:axId val="-2078126592"/>
+        <c:axId val="-2078132848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2078906496"/>
+        <c:axId val="-2078126592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078953424"/>
+        <c:crossAx val="-2078132848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2078953424"/>
+        <c:axId val="-2078132848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078906496"/>
+        <c:crossAx val="-2078126592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3360,16 +3357,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3355</c:v>
+                    <c:v>0.3499</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.2799</c:v>
+                    <c:v>5.8325</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3457</c:v>
+                    <c:v>8.1372</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3673</c:v>
+                    <c:v>1.7246</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3384,16 +3381,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.0859</c:v>
+                    <c:v>1.1405</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>8.729</c:v>
+                    <c:v>8.9604</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.296</c:v>
+                    <c:v>6.5452</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.2852</c:v>
+                    <c:v>0.3937</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3446,16 +3443,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0955</c:v>
+                  <c:v>23.041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.9385</c:v>
+                  <c:v>62.5123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65.4849</c:v>
+                  <c:v>65.9781</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.5552</c:v>
+                  <c:v>81.7638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3510,13 +3507,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.281000000000001</c:v>
+                    <c:v>9.5636</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.9835</c:v>
+                    <c:v>13.1658</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2442</c:v>
+                    <c:v>2.1987</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3534,13 +3531,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>15.1292</c:v>
+                    <c:v>15.9118</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.025</c:v>
+                    <c:v>2.2477</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.4389</c:v>
+                    <c:v>0.8538</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3596,13 +3593,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.8892</c:v>
+                  <c:v>38.594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.0713</c:v>
+                  <c:v>39.6419</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.9683</c:v>
+                  <c:v>66.2199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,13 +3654,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>13.5781</c:v>
+                    <c:v>14.4625</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>19.328</c:v>
+                    <c:v>21.1739</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.874</c:v>
+                    <c:v>12.3329</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3681,13 +3678,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.5978</c:v>
+                    <c:v>8.0676</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.3007</c:v>
+                    <c:v>17.5378</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.8664</c:v>
+                    <c:v>2.6872</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3743,13 +3740,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.5978</c:v>
+                  <c:v>8.0676</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1816</c:v>
+                  <c:v>2.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.9479</c:v>
+                  <c:v>40.4913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,10 +3804,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.8061</c:v>
+                    <c:v>7.275</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>15.6414</c:v>
+                    <c:v>14.4494</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3831,10 +3828,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>43.8311</c:v>
+                    <c:v>31.4348</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>10.5393</c:v>
+                    <c:v>10.9984</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3893,10 +3890,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.1912</c:v>
+                  <c:v>0.1156</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0195</c:v>
+                  <c:v>7.3124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079942640"/>
-        <c:axId val="-2080342720"/>
+        <c:axId val="-2078191600"/>
+        <c:axId val="-2078197856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079942640"/>
+        <c:axId val="-2078191600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080342720"/>
+        <c:crossAx val="-2078197856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080342720"/>
+        <c:axId val="-2078197856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079942640"/>
+        <c:crossAx val="-2078191600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>0</v>
-          </cell>
-          <cell r="G4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>17.238099999999999</v>
-          </cell>
-          <cell r="F5">
-            <v>0.85809999999999997</v>
-          </cell>
-          <cell r="G5">
-            <v>0.26169999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>39.0169</v>
-          </cell>
-          <cell r="F6">
-            <v>5.5888</v>
-          </cell>
-          <cell r="G6">
-            <v>3.5430000000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>37.366900000000001</v>
-          </cell>
-          <cell r="F7">
-            <v>0.45179999999999998</v>
-          </cell>
-          <cell r="G7">
-            <v>3.6985999999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>43.737499999999997</v>
-          </cell>
-          <cell r="F8">
-            <v>0.55379999999999996</v>
-          </cell>
-          <cell r="G8">
-            <v>0.62960000000000005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-          <cell r="F10">
-            <v>0.14960000000000001</v>
-          </cell>
-          <cell r="G10">
-            <v>0.1321</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>0</v>
-          </cell>
-          <cell r="G11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>29.504799999999999</v>
-          </cell>
-          <cell r="F12">
-            <v>11.3765</v>
-          </cell>
-          <cell r="G12">
-            <v>7.0321999999999996</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>25.740200000000002</v>
-          </cell>
-          <cell r="F13">
-            <v>6.4233000000000002</v>
-          </cell>
-          <cell r="G13">
-            <v>8.2149999999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>38.281599999999997</v>
-          </cell>
-          <cell r="F14">
-            <v>4.1418999999999997</v>
-          </cell>
-          <cell r="G14">
-            <v>3.6036999999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>5.67E-2</v>
-          </cell>
-          <cell r="G16">
-            <v>5.5399999999999998E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>0</v>
-          </cell>
-          <cell r="G17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>21.405999999999999</v>
-          </cell>
-          <cell r="F18">
-            <v>17.685300000000002</v>
-          </cell>
-          <cell r="G18">
-            <v>11.0158</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>11.6884</v>
-          </cell>
-          <cell r="F19">
-            <v>1.7146999999999999</v>
-          </cell>
-          <cell r="G19">
-            <v>13.567500000000001</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>30.694099999999999</v>
-          </cell>
-          <cell r="F20">
-            <v>1.4945999999999999</v>
-          </cell>
-          <cell r="G20">
-            <v>0.9889</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>0</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>20.959399999999999</v>
-          </cell>
-          <cell r="F24">
-            <v>17.539000000000001</v>
-          </cell>
-          <cell r="G24">
-            <v>11.4734</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>11.173999999999999</v>
-          </cell>
-          <cell r="F25">
-            <v>1.6026</v>
-          </cell>
-          <cell r="G25">
-            <v>15.063000000000001</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>30.448599999999999</v>
-          </cell>
-          <cell r="F26">
-            <v>1.0718000000000001</v>
-          </cell>
-          <cell r="G26">
-            <v>1.0788</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F29">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G29">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>21.983799999999999</v>
-          </cell>
-          <cell r="F30">
-            <v>0</v>
-          </cell>
-          <cell r="G30">
-            <v>1.04E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>35.973199999999999</v>
-          </cell>
-          <cell r="F31">
-            <v>1.41E-2</v>
-          </cell>
-          <cell r="G31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>43.386400000000002</v>
-          </cell>
-          <cell r="F32">
-            <v>1.0591999999999999</v>
-          </cell>
-          <cell r="G32">
-            <v>0.31219999999999998</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>46.470100000000002</v>
-          </cell>
-          <cell r="F33">
-            <v>0.31119999999999998</v>
-          </cell>
-          <cell r="G33">
-            <v>0.73719999999999997</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>0.66649999999999998</v>
-          </cell>
-          <cell r="F35">
-            <v>6.0900000000000003E-2</v>
-          </cell>
-          <cell r="G35">
-            <v>7.1099999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>-3.3066</v>
-          </cell>
-          <cell r="F36">
-            <v>1.4800000000000001E-2</v>
-          </cell>
-          <cell r="G36">
-            <v>4.3499999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>23.038799999999998</v>
-          </cell>
-          <cell r="F37">
-            <v>1.9400000000000001E-2</v>
-          </cell>
-          <cell r="G37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>36.491900000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>0.39829999999999999</v>
-          </cell>
-          <cell r="G38">
-            <v>4.1999999999999997E-3</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>43.240400000000001</v>
-          </cell>
-          <cell r="F39">
-            <v>0.32119999999999999</v>
-          </cell>
-          <cell r="G39">
-            <v>0.2445</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>5.5399999999999998E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>-25.8263</v>
-          </cell>
-          <cell r="F42">
-            <v>0.14069999999999999</v>
-          </cell>
-          <cell r="G42">
-            <v>0.41310000000000002</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>4.2622999999999998</v>
-          </cell>
-          <cell r="F43">
-            <v>6.3799999999999996E-2</v>
-          </cell>
-          <cell r="G43">
-            <v>2.9399999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>26.016400000000001</v>
-          </cell>
-          <cell r="F44">
-            <v>0.78810000000000002</v>
-          </cell>
-          <cell r="G44">
-            <v>1.8937999999999999</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>38.520299999999999</v>
-          </cell>
-          <cell r="F45">
-            <v>1.2095</v>
-          </cell>
-          <cell r="G45">
-            <v>1.2844</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>3.2288999999999999</v>
-          </cell>
-          <cell r="F48">
-            <v>3.9399999999999998E-2</v>
-          </cell>
-          <cell r="G48">
-            <v>1.34E-2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>2.8248000000000002</v>
-          </cell>
-          <cell r="F49">
-            <v>1.72E-2</v>
-          </cell>
-          <cell r="G49">
-            <v>0.2344</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>25.581399999999999</v>
-          </cell>
-          <cell r="F50">
-            <v>0.81010000000000004</v>
-          </cell>
-          <cell r="G50">
-            <v>2.3727999999999998</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>37.437899999999999</v>
-          </cell>
-          <cell r="F51">
-            <v>0.39140000000000003</v>
-          </cell>
-          <cell r="G51">
-            <v>0.64049999999999996</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F54">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G54">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>39.221800000000002</v>
-          </cell>
-          <cell r="F55">
-            <v>0.83879999999999999</v>
-          </cell>
-          <cell r="G55">
-            <v>0.26179999999999998</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>74.990200000000002</v>
-          </cell>
-          <cell r="F56">
-            <v>5.5888999999999998</v>
-          </cell>
-          <cell r="G56">
-            <v>3.3452000000000002</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>81.661600000000007</v>
-          </cell>
-          <cell r="F57">
-            <v>1.395</v>
-          </cell>
-          <cell r="G57">
-            <v>2.9843000000000002</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>90.127700000000004</v>
-          </cell>
-          <cell r="F58">
-            <v>0.27150000000000002</v>
-          </cell>
-          <cell r="G58">
-            <v>0.8458</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>0.66649999999999998</v>
-          </cell>
-          <cell r="F60">
-            <v>6.0900000000000003E-2</v>
-          </cell>
-          <cell r="G60">
-            <v>7.1099999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>-3.3066</v>
-          </cell>
-          <cell r="F61">
-            <v>1.4800000000000001E-2</v>
-          </cell>
-          <cell r="G61">
-            <v>4.3499999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>52.543500000000002</v>
-          </cell>
-          <cell r="F62">
-            <v>11.3764</v>
-          </cell>
-          <cell r="G62">
-            <v>7.0129000000000001</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>64.343500000000006</v>
-          </cell>
-          <cell r="F63">
-            <v>3.3269000000000002</v>
-          </cell>
-          <cell r="G63">
-            <v>2.9885999999999999</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>81.229100000000003</v>
-          </cell>
-          <cell r="F64">
-            <v>0.6744</v>
-          </cell>
-          <cell r="G64">
-            <v>1.0382</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0</v>
-          </cell>
-          <cell r="F66">
-            <v>0</v>
-          </cell>
-          <cell r="G66">
-            <v>5.5399999999999998E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>-25.8263</v>
-          </cell>
-          <cell r="F67">
-            <v>0.14069999999999999</v>
-          </cell>
-          <cell r="G67">
-            <v>0.41310000000000002</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>25.697700000000001</v>
-          </cell>
-          <cell r="F68">
-            <v>17.690899999999999</v>
-          </cell>
-          <cell r="G68">
-            <v>11.010199999999999</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>38.745600000000003</v>
-          </cell>
-          <cell r="F69">
-            <v>2.1747999999999998</v>
-          </cell>
-          <cell r="G69">
-            <v>12.9907</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>68.383600000000001</v>
-          </cell>
-          <cell r="F70">
-            <v>0.80510000000000004</v>
-          </cell>
-          <cell r="G70">
-            <v>0.6915</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>3.2288999999999999</v>
-          </cell>
-          <cell r="F73">
-            <v>3.9399999999999998E-2</v>
-          </cell>
-          <cell r="G73">
-            <v>1.34E-2</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>23.784099999999999</v>
-          </cell>
-          <cell r="F74">
-            <v>17.5532</v>
-          </cell>
-          <cell r="G74">
-            <v>11.456300000000001</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>43.014899999999997</v>
-          </cell>
-          <cell r="F75">
-            <v>7.9104000000000001</v>
-          </cell>
-          <cell r="G75">
-            <v>7.6696</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>67.875100000000003</v>
-          </cell>
-          <cell r="F76">
-            <v>4.5377000000000001</v>
-          </cell>
-          <cell r="G76">
-            <v>2.0217000000000001</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>22.095500000000001</v>
-          </cell>
-          <cell r="F80">
-            <v>1.0859000000000001</v>
-          </cell>
-          <cell r="G80">
-            <v>0.33550000000000002</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>60.938499999999998</v>
-          </cell>
-          <cell r="F81">
-            <v>8.7289999999999992</v>
-          </cell>
-          <cell r="G81">
-            <v>5.2321</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>67.6066</v>
-          </cell>
-          <cell r="F82">
-            <v>2.4064999999999999</v>
-          </cell>
-          <cell r="G82">
-            <v>5.2725</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>81.592200000000005</v>
-          </cell>
-          <cell r="F83">
-            <v>0.79159999999999997</v>
-          </cell>
-          <cell r="G83">
-            <v>1.5986</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>38.337200000000003</v>
-          </cell>
-          <cell r="F87">
-            <v>14.7821</v>
-          </cell>
-          <cell r="G87">
-            <v>9.1254000000000008</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>43.852800000000002</v>
-          </cell>
-          <cell r="F88">
-            <v>5.2386999999999997</v>
-          </cell>
-          <cell r="G88">
-            <v>4.7081999999999997</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>66.929000000000002</v>
-          </cell>
-          <cell r="F89">
-            <v>1.3363</v>
-          </cell>
-          <cell r="G89">
-            <v>2.0049999999999999</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>22.3659</v>
-          </cell>
-          <cell r="F93">
-            <v>18.4389</v>
-          </cell>
-          <cell r="G93">
-            <v>11.5077</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>17.4054</v>
-          </cell>
-          <cell r="F94">
-            <v>4.0247000000000002</v>
-          </cell>
-          <cell r="G94">
-            <v>18.046500000000002</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>48.574199999999998</v>
-          </cell>
-          <cell r="F95">
-            <v>1.6625000000000001</v>
-          </cell>
-          <cell r="G95">
-            <v>0.30649999999999999</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>21.5686</v>
-          </cell>
-          <cell r="F99">
-            <v>18.154699999999998</v>
-          </cell>
-          <cell r="G99">
-            <v>11.6281</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>20.904399999999999</v>
-          </cell>
-          <cell r="F100">
-            <v>8.2058</v>
-          </cell>
-          <cell r="G100">
-            <v>12.692</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>48.7271</v>
-          </cell>
-          <cell r="F101">
-            <v>7.3289</v>
-          </cell>
-          <cell r="G101">
-            <v>3.1459999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7785,8 +6873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="R90" sqref="R90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1.03E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>17.238099999999999</v>
+        <v>16.805700000000002</v>
       </c>
       <c r="F5">
-        <v>0.85809999999999997</v>
+        <v>0.82169999999999999</v>
       </c>
       <c r="G5">
-        <v>0.26169999999999999</v>
+        <v>0.25519999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7902,7 +6990,7 @@
         <v>5.5888</v>
       </c>
       <c r="G6">
-        <v>3.6522999999999999</v>
+        <v>3.508</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>37.7652</v>
+        <v>39.739600000000003</v>
       </c>
       <c r="F7">
-        <v>0.91710000000000003</v>
+        <v>2.4742999999999999</v>
       </c>
       <c r="G7">
-        <v>3.9735</v>
+        <v>1.7931999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>43.6539</v>
+        <v>43.687399999999997</v>
       </c>
       <c r="F8">
-        <v>0.1651</v>
+        <v>0.4476</v>
       </c>
       <c r="G8">
-        <v>1.8986000000000001</v>
+        <v>1.2095</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7968,10 +7056,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.26300000000000001</v>
+        <v>5.8900000000000001E-2</v>
       </c>
       <c r="G10">
-        <v>0.19209999999999999</v>
+        <v>0.23499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7991,10 +7079,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G11">
-        <v>0.13550000000000001</v>
+        <v>3.9300000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>28.887499999999999</v>
+        <v>28.0718</v>
       </c>
       <c r="F12">
-        <v>11.911099999999999</v>
+        <v>11.4278</v>
       </c>
       <c r="G12">
-        <v>7.1414999999999997</v>
+        <v>7.1593</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>24.7256</v>
+        <v>27.957000000000001</v>
       </c>
       <c r="F13">
-        <v>1.6279999999999999</v>
+        <v>4.5724999999999998</v>
       </c>
       <c r="G13">
-        <v>12.668100000000001</v>
+        <v>5.4943999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>37.367199999999997</v>
+        <v>36.690899999999999</v>
       </c>
       <c r="F14">
-        <v>0.79590000000000005</v>
+        <v>2.6208999999999998</v>
       </c>
       <c r="G14">
-        <v>2.649</v>
+        <v>1.7788999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8086,7 +7174,7 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0.1724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8106,10 +7194,10 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.24340000000000001</v>
+        <v>0.28710000000000002</v>
       </c>
       <c r="G17">
-        <v>0.26779999999999998</v>
+        <v>0.57350000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>8.0200999999999993</v>
+        <v>6.9203999999999999</v>
       </c>
       <c r="F18">
-        <v>8.0200999999999993</v>
+        <v>6.9203999999999999</v>
       </c>
       <c r="G18">
-        <v>14.3773</v>
+        <v>12.0045</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>3.4820000000000002</v>
+        <v>0.67069999999999996</v>
       </c>
       <c r="F19">
-        <v>7.3723000000000001</v>
+        <v>3.3494000000000002</v>
       </c>
       <c r="G19">
-        <v>12.925599999999999</v>
+        <v>17.5504</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>24.358799999999999</v>
+        <v>24.143899999999999</v>
       </c>
       <c r="F20">
-        <v>5.7351999999999999</v>
+        <v>6.0858999999999996</v>
       </c>
       <c r="G20">
-        <v>2.1141000000000001</v>
+        <v>1.3939999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8221,7 +7309,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.1153</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -8241,13 +7329,13 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>-2.86E-2</v>
+        <v>3.7199999999999997E-2</v>
       </c>
       <c r="F24">
-        <v>0.2611</v>
+        <v>0.30609999999999998</v>
       </c>
       <c r="G24">
-        <v>0.21970000000000001</v>
+        <v>0.13250000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>-22.630199999999999</v>
+        <v>-12.326700000000001</v>
       </c>
       <c r="F25">
-        <v>7.0137999999999998</v>
+        <v>13.603999999999999</v>
       </c>
       <c r="G25">
-        <v>46.412399999999998</v>
+        <v>23.681000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>2.1263999999999998</v>
+        <v>0.91349999999999998</v>
       </c>
       <c r="F26">
-        <v>2.6492</v>
+        <v>3.9685999999999999</v>
       </c>
       <c r="G26">
-        <v>10.610300000000001</v>
+        <v>7.43</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>-3.8346</v>
+        <v>10.898199999999999</v>
       </c>
       <c r="F29">
-        <v>0.52749999999999997</v>
+        <v>0.2646</v>
       </c>
       <c r="G29">
-        <v>0.10730000000000001</v>
+        <v>1.3318000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7429,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>21.983799999999999</v>
+        <v>27.025200000000002</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>1.04E-2</v>
+        <v>2.92E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,10 +7452,10 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>35.973199999999999</v>
+        <v>37.578200000000002</v>
       </c>
       <c r="F31">
-        <v>1.41E-2</v>
+        <v>1.04E-2</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>43.075600000000001</v>
+        <v>44.125900000000001</v>
       </c>
       <c r="F32">
-        <v>8.9700000000000002E-2</v>
+        <v>0.34329999999999999</v>
       </c>
       <c r="G32">
-        <v>0.45300000000000001</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>46.816899999999997</v>
+        <v>47.264200000000002</v>
       </c>
       <c r="F33">
-        <v>0.60450000000000004</v>
+        <v>0.49730000000000002</v>
       </c>
       <c r="G33">
-        <v>0.50980000000000003</v>
+        <v>0.65310000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>0.3841</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="F35">
-        <v>0.19589999999999999</v>
+        <v>3.6700000000000003E-2</v>
       </c>
       <c r="G35">
-        <v>7.7299999999999994E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>-5.0045000000000002</v>
+        <v>13.8269</v>
       </c>
       <c r="F36">
-        <v>3.7900000000000003E-2</v>
+        <v>0.16059999999999999</v>
       </c>
       <c r="G36">
-        <v>0.12720000000000001</v>
+        <v>8.8200000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,13 +7567,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>21.983799999999999</v>
+        <v>27.124400000000001</v>
       </c>
       <c r="F37">
-        <v>0.1396</v>
+        <v>0.2354</v>
       </c>
       <c r="G37">
-        <v>0.1087</v>
+        <v>8.5000000000000006E-3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>35.933900000000001</v>
+        <v>37.564999999999998</v>
       </c>
       <c r="F38">
-        <v>0.15570000000000001</v>
+        <v>0.25080000000000002</v>
       </c>
       <c r="G38">
-        <v>0.6431</v>
+        <v>0.7913</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>43.1629</v>
+        <v>43.832700000000003</v>
       </c>
       <c r="F39">
-        <v>0.13739999999999999</v>
+        <v>0.31590000000000001</v>
       </c>
       <c r="G39">
-        <v>0.37040000000000001</v>
+        <v>0.38350000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8554,7 +7642,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0.1724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8574,10 +7662,10 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="F42">
-        <v>2.86E-2</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="G42">
-        <v>0.2636</v>
+        <v>0.57320000000000004</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>-5.7415000000000003</v>
+        <v>15.578099999999999</v>
       </c>
       <c r="F43">
-        <v>0.19089999999999999</v>
+        <v>1.8051999999999999</v>
       </c>
       <c r="G43">
-        <v>0.74450000000000005</v>
+        <v>9.9199999999999997E-2</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>21.6325</v>
+        <v>27.256399999999999</v>
       </c>
       <c r="F44">
-        <v>12.7317</v>
+        <v>1.1657</v>
       </c>
       <c r="G44">
-        <v>2.7587999999999999</v>
+        <v>1.1251</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>36.095399999999998</v>
+        <v>37.859900000000003</v>
       </c>
       <c r="F45">
-        <v>0.41839999999999999</v>
+        <v>0.53710000000000002</v>
       </c>
       <c r="G45">
-        <v>0.28089999999999998</v>
+        <v>0.1123</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>0.33560000000000001</v>
+        <v>0.35859999999999997</v>
       </c>
       <c r="F49">
-        <v>9.2899999999999996E-2</v>
+        <v>0.1028</v>
       </c>
       <c r="G49">
-        <v>0.40639999999999998</v>
+        <v>0.16930000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>-8.2013999999999996</v>
+        <v>8.2472999999999992</v>
       </c>
       <c r="F50">
-        <v>42.866500000000002</v>
+        <v>22.586500000000001</v>
       </c>
       <c r="G50">
-        <v>5.8691000000000004</v>
+        <v>6.5406000000000004</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>21.259899999999998</v>
+        <v>26.967099999999999</v>
       </c>
       <c r="F51">
-        <v>9.0968999999999998</v>
+        <v>1.1904999999999999</v>
       </c>
       <c r="G51">
-        <v>2.1303999999999998</v>
+        <v>7.7694999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>-3.8346</v>
+        <v>10.898199999999999</v>
       </c>
       <c r="F54">
-        <v>0.52749999999999997</v>
+        <v>0.2646</v>
       </c>
       <c r="G54">
-        <v>0.10730000000000001</v>
+        <v>1.3318000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>39.221800000000002</v>
+        <v>43.839300000000001</v>
       </c>
       <c r="F55">
-        <v>0.83879999999999999</v>
+        <v>0.80940000000000001</v>
       </c>
       <c r="G55">
-        <v>0.26179999999999998</v>
+        <v>0.25530000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>74.990200000000002</v>
+        <v>76.599500000000006</v>
       </c>
       <c r="F56">
-        <v>5.5888999999999998</v>
+        <v>5.5932000000000004</v>
       </c>
       <c r="G56">
-        <v>3.3757999999999999</v>
+        <v>3.6374</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>80.340999999999994</v>
+        <v>81.057900000000004</v>
       </c>
       <c r="F57">
-        <v>2.9379</v>
+        <v>3.3203999999999998</v>
       </c>
       <c r="G57">
-        <v>4.26</v>
+        <v>4.4546999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>90.113900000000001</v>
+        <v>90.502099999999999</v>
       </c>
       <c r="F58">
-        <v>1.6204000000000001</v>
+        <v>0.25829999999999997</v>
       </c>
       <c r="G58">
-        <v>0.89080000000000004</v>
+        <v>0.78239999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>0.3841</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="F60">
-        <v>0.19589999999999999</v>
+        <v>3.6700000000000003E-2</v>
       </c>
       <c r="G60">
-        <v>7.7299999999999994E-2</v>
+        <v>7.0499999999999993E-2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>-5.0045000000000002</v>
+        <v>13.8269</v>
       </c>
       <c r="F61">
-        <v>3.7900000000000003E-2</v>
+        <v>0.16059999999999999</v>
       </c>
       <c r="G61">
-        <v>0.12720000000000001</v>
+        <v>8.8200000000000001E-2</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>50.832000000000001</v>
+        <v>55.105499999999999</v>
       </c>
       <c r="F62">
-        <v>11.8719</v>
+        <v>11.444699999999999</v>
       </c>
       <c r="G62">
-        <v>7.1719999999999997</v>
+        <v>7.1140999999999996</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>64.251800000000003</v>
+        <v>62.1858</v>
       </c>
       <c r="F63">
-        <v>3.6684999999999999</v>
+        <v>1.1454</v>
       </c>
       <c r="G63">
-        <v>5.6044</v>
+        <v>8.3497000000000003</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>80.218699999999998</v>
+        <v>81.070899999999995</v>
       </c>
       <c r="F64">
-        <v>3.2532000000000001</v>
+        <v>0.63319999999999999</v>
       </c>
       <c r="G64">
-        <v>2.5999999999999999E-2</v>
+        <v>1.1585000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9022,7 +8110,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>0.1724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9042,10 +8130,10 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="F67">
-        <v>2.86E-2</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="G67">
-        <v>0.2636</v>
+        <v>0.57320000000000004</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>2.2519</v>
+        <v>22.4802</v>
       </c>
       <c r="F68">
-        <v>7.2564000000000002</v>
+        <v>8.7073</v>
       </c>
       <c r="G68">
-        <v>14.3772</v>
+        <v>12.0412</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>24.073699999999999</v>
+        <v>28.4252</v>
       </c>
       <c r="F69">
-        <v>4.8856000000000002</v>
+        <v>13.626200000000001</v>
       </c>
       <c r="G69">
-        <v>14.556699999999999</v>
+        <v>16.7393</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>61.642499999999998</v>
+        <v>63.006799999999998</v>
       </c>
       <c r="F70">
-        <v>2.1135999999999999</v>
+        <v>1.6012999999999999</v>
       </c>
       <c r="G70">
-        <v>3.7351999999999999</v>
+        <v>7.6780999999999997</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>0.33560000000000001</v>
+        <v>0.35859999999999997</v>
       </c>
       <c r="F74">
-        <v>9.2899999999999996E-2</v>
+        <v>0.1028</v>
       </c>
       <c r="G74">
-        <v>0.40639999999999998</v>
+        <v>0.16930000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>-15.534700000000001</v>
+        <v>-5.5627000000000004</v>
       </c>
       <c r="F75">
-        <v>21.0212</v>
+        <v>8.7211999999999996</v>
       </c>
       <c r="G75">
-        <v>45.945999999999998</v>
+        <v>20.170300000000001</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>21.519100000000002</v>
+        <v>32.331000000000003</v>
       </c>
       <c r="F76">
-        <v>11.7506</v>
+        <v>5.2018000000000004</v>
       </c>
       <c r="G76">
-        <v>3.4872999999999998</v>
+        <v>10.466900000000001</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,13 +8362,13 @@
         <v>4</v>
       </c>
       <c r="E80">
-        <v>22.095500000000001</v>
+        <v>23.041</v>
       </c>
       <c r="F80">
-        <v>1.0859000000000001</v>
+        <v>1.1405000000000001</v>
       </c>
       <c r="G80">
-        <v>0.33550000000000002</v>
+        <v>0.34989999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>60.938499999999998</v>
+        <v>62.512300000000003</v>
       </c>
       <c r="F81">
-        <v>8.7289999999999992</v>
+        <v>8.9603999999999999</v>
       </c>
       <c r="G81">
-        <v>5.2798999999999996</v>
+        <v>5.8324999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>65.484899999999996</v>
+        <v>65.978099999999998</v>
       </c>
       <c r="F82">
-        <v>5.2960000000000003</v>
+        <v>6.5452000000000004</v>
       </c>
       <c r="G82">
-        <v>7.3456999999999999</v>
+        <v>8.1372</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>81.555199999999999</v>
+        <v>81.763800000000003</v>
       </c>
       <c r="F83">
-        <v>3.2852000000000001</v>
+        <v>0.39369999999999999</v>
       </c>
       <c r="G83">
-        <v>1.3673</v>
+        <v>1.7245999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,13 +8500,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>36.889200000000002</v>
+        <v>38.594000000000001</v>
       </c>
       <c r="F87">
-        <v>15.129200000000001</v>
+        <v>15.911799999999999</v>
       </c>
       <c r="G87">
-        <v>9.2810000000000006</v>
+        <v>9.5635999999999992</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>44.071300000000001</v>
+        <v>39.6419</v>
       </c>
       <c r="F88">
-        <v>6.0250000000000004</v>
+        <v>2.2477</v>
       </c>
       <c r="G88">
-        <v>8.9834999999999994</v>
+        <v>13.165800000000001</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>64.968299999999999</v>
+        <v>66.219899999999996</v>
       </c>
       <c r="F89">
-        <v>5.4389000000000003</v>
+        <v>0.8538</v>
       </c>
       <c r="G89">
-        <v>0.2442</v>
+        <v>2.1987000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8615,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>7.5978000000000003</v>
+        <v>8.0676000000000005</v>
       </c>
       <c r="F93">
-        <v>7.5978000000000003</v>
+        <v>8.0676000000000005</v>
       </c>
       <c r="G93">
-        <v>13.578099999999999</v>
+        <v>14.4625</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>4.1816000000000004</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="F94">
-        <v>7.3007</v>
+        <v>17.537800000000001</v>
       </c>
       <c r="G94">
-        <v>19.327999999999999</v>
+        <v>21.1739</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>39.947899999999997</v>
+        <v>40.491300000000003</v>
       </c>
       <c r="F95">
-        <v>2.8664000000000001</v>
+        <v>2.6871999999999998</v>
       </c>
       <c r="G95">
-        <v>5.8739999999999997</v>
+        <v>12.3329</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>13.1912</v>
+        <v>0.11559999999999999</v>
       </c>
       <c r="F100">
-        <v>43.831099999999999</v>
+        <v>31.434799999999999</v>
       </c>
       <c r="G100">
-        <v>18.806100000000001</v>
+        <v>7.2750000000000004</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>-1.0195000000000001</v>
+        <v>7.3124000000000002</v>
       </c>
       <c r="F101">
-        <v>10.539300000000001</v>
+        <v>10.9984</v>
       </c>
       <c r="G101">
-        <v>15.641400000000001</v>
+        <v>14.449400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>